<commit_message>
remove some unnecessary files
</commit_message>
<xml_diff>
--- a/Leetcode-tag record.xlsx
+++ b/Leetcode-tag record.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chiahsing/Mission-Impossible/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8C0C055-33DA-9043-A027-9BE27813D8E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FB39E5B-85ED-AA40-920B-E0210A059AAE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12740" yWindow="4120" windowWidth="46140" windowHeight="23100" activeTab="1" xr2:uid="{073527F3-3865-0D40-BFED-DB63B5BC01C0}"/>
+    <workbookView xWindow="12740" yWindow="4100" windowWidth="46140" windowHeight="23100" activeTab="1" xr2:uid="{073527F3-3865-0D40-BFED-DB63B5BC01C0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
New interview coding questions category added
</commit_message>
<xml_diff>
--- a/Leetcode-tag record.xlsx
+++ b/Leetcode-tag record.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chiahsing/Mission-Impossible/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F23878F-DA9B-B541-89E7-DF0D7AF38045}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BE2F375-4565-7549-B34D-880C72509A94}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4000" yWindow="12720" windowWidth="53180" windowHeight="19600" activeTab="1" xr2:uid="{073527F3-3865-0D40-BFED-DB63B5BC01C0}"/>
+    <workbookView xWindow="6220" yWindow="3780" windowWidth="53180" windowHeight="19600" activeTab="1" xr2:uid="{073527F3-3865-0D40-BFED-DB63B5BC01C0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>